<commit_message>
Using google maps to get coordinates 🗺
</commit_message>
<xml_diff>
--- a/linhas/Linha 0903.xlsx
+++ b/linhas/Linha 0903.xlsx
@@ -50,9 +50,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -418,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A60"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,6 +430,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="150" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -435,6 +440,16 @@
           <t>Linha 0903 - T.I. Benedito Bentes / Eustáquio Gomes (Via Forene)</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Latitude</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Longitude</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -442,6 +457,12 @@
           <t>Terminal Benedito Bentes (Desembarque)</t>
         </is>
       </c>
+      <c r="B2" s="2" t="n">
+        <v>-9.549443999999999</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>-35.72652</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -449,6 +470,12 @@
           <t>Avenida Benedito Bentes 1768-1862 - Benedito Bentes Maceió - Al 57084-800 República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B3" s="2" t="n">
+        <v>-9.5476425</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>-35.7293331</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -456,6 +483,12 @@
           <t>Av. Cachoeira Do Meirim 1311-1379 - Benedito Bentes Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B4" s="2" t="n">
+        <v>-9.549807899999999</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>-35.7331086</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -463,6 +496,12 @@
           <t>Avenida Cachoeira Do Meirim 935-981 - Benedito Bentes Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B5" s="2" t="n">
+        <v>-9.5520394</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>-35.7353938</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -470,6 +509,12 @@
           <t>Al-105 531-617 - Benedito Bentes Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B6" s="2" t="n">
+        <v>-9.160664499999999</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>-35.5350591</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -477,6 +522,12 @@
           <t>Avenida Cachoeira Do Meirim 217-333 - Benedito Bentes Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B7" s="2" t="n">
+        <v>-9.556360699999999</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>-35.7399394</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -484,6 +535,12 @@
           <t>Avenida Cachoeira Do Meirim 629-685 Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B8" s="2" t="n">
+        <v>-9.5580718</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>-35.74165929999999</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -491,6 +548,12 @@
           <t>Av. Cachoeira Do Meirim 398-462 - Antares Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B9" s="2" t="n">
+        <v>-9.559123999999999</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>-35.7427718</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -498,6 +561,12 @@
           <t>Av. Cachoeira Do Meirim 183-297 - Antares Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B10" s="2" t="n">
+        <v>-9.560942499999999</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>-35.7448797</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -505,6 +574,12 @@
           <t>Avenida Menino Marcelo 7014-7654 - Tabuleiro Do Martins Maceió - Al 57081-385 República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B11" s="2" t="n">
+        <v>-9.5613946</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>-35.74615989999999</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -512,6 +587,12 @@
           <t>Br-316 7014-7654 - Tabuleiro Do Martins Maceió - Al 57081-385 República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B12" s="2" t="n">
+        <v>-9.565182399999999</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>-35.777396</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -519,6 +600,12 @@
           <t>Avenida Empresário Nelson Oliveira Menezes 1459 - Cidade Universitária Maceió - Al 57073-471 República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B13" s="2" t="n">
+        <v>-9.546670300000001</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>-35.7462117</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -526,6 +613,12 @@
           <t>Avenida Empresário Nelson Oliveira Menezes 1201-1289 - Cidade Universitária Maceió - Al República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B14" s="2" t="n">
+        <v>-9.547639199999999</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>-35.7478589</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -533,6 +626,12 @@
           <t>Av. Empresário Nelson Oliveira Menezes 963 - Cidade Universitária Maceió - Al 57073-471 Brasil</t>
         </is>
       </c>
+      <c r="B15" s="2" t="n">
+        <v>-9.5487631</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>-35.7502234</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -540,6 +639,12 @@
           <t>Rue 16 210-260 - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B16" s="2" t="n">
+        <v>-9.549141199999999</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>-35.7518819</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -547,6 +652,12 @@
           <t>Av. Tancredo Neves 1552 - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B17" s="2" t="n">
+        <v>-9.5485849</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>-35.75471599999999</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -554,6 +665,12 @@
           <t>Av. Tancredo Neves 1736-1796 - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B18" s="2" t="n">
+        <v>-9.547731799999999</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>-35.7532515</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -561,6 +678,12 @@
           <t>Rua Padre Cícero 102 - Cidade Universitária Maceió - Al República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B19" s="2" t="n">
+        <v>-9.546125</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>-35.7526961</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -575,6 +698,12 @@
           <t>Av. Benedito Loureiro 1004-1062 - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B21" s="2" t="n">
+        <v>-9.542885099999999</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>-35.7528852</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -582,6 +711,12 @@
           <t>Av. Tancredo Neves 52-60 - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B22" s="2" t="n">
+        <v>-9.547007499999999</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>-35.7520547</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -589,6 +724,12 @@
           <t>Avenida Tancredo Neves 773-803 - Cidade Universitária Maceió - Al República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B23" s="2" t="n">
+        <v>-9.5392022</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>-35.7541773</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -596,6 +737,12 @@
           <t>Rua São Pedro 860-960 - Cidade Universitária Maceió - Al República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B24" s="2" t="n">
+        <v>-9.539851499999999</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>-35.7560938</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -603,6 +750,12 @@
           <t>R. São Pedro 826-858 - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B25" s="2" t="n">
+        <v>-9.5399694</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>-35.7563304</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -624,6 +777,12 @@
           <t>Rua Senador Arnon De Melo 430-540 - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B28" s="2" t="n">
+        <v>-9.5416533</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>-35.7595592</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -631,6 +790,12 @@
           <t>Terminal Village Campestre</t>
         </is>
       </c>
+      <c r="B29" s="2" t="n">
+        <v>18.3654432</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>-66.13259719999999</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -638,6 +803,12 @@
           <t>Av. Alice Carolina 07 - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B30" s="2" t="n">
+        <v>-9.5505864</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>-35.7593578</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -645,6 +816,12 @@
           <t>Travassa Hailton Dos Santos 180 - Cidade Universitária Maceió - Al 57073-480 República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B31" s="2" t="n">
+        <v>-9.5516975</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>-35.7612876</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -652,6 +829,12 @@
           <t>Travassa Hailton Dos Santos 404-458 - Cidade Universitária Maceió - Al 57073-480 República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B32" s="2" t="n">
+        <v>-9.5474643</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>-35.754939</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -659,6 +842,12 @@
           <t>Travassa Hailton Dos Santos 662-700 - Cidade Universitária Maceió - Al 57073-480 República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B33" s="2" t="n">
+        <v>-9.5470734</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>-35.7542347</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -666,6 +855,12 @@
           <t>Travassa Hailton Dos Santos 30 - Cidade Universitária Maceió - Al 57073-480 República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B34" s="2" t="n">
+        <v>-9.5500852</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>-35.7592794</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -673,6 +868,12 @@
           <t>Universidade Federal De Alagoas - Unnamed Road - Cidade Universitária Maceió - Al República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B35" s="2" t="n">
+        <v>-9.5435246</v>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>-35.7627701</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -680,6 +881,12 @@
           <t>Universidade Federal De Alagoas - Unnamed Road - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B36" s="2" t="n">
+        <v>-9.552133999999999</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>-35.77124999999999</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -687,6 +894,12 @@
           <t>Universidade Federal De Alagoas - Unnamed Road - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B37" s="2" t="n">
+        <v>-9.552133999999999</v>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>-35.77124999999999</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -694,6 +907,12 @@
           <t>Universidade Federal De Alagoas - Unnamed Road - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B38" s="2" t="n">
+        <v>-9.552133999999999</v>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>-35.77124999999999</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -701,6 +920,12 @@
           <t>Unnamed Road - Universidade Federal De Alagoas Cidade Universitária Maceió - Al República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B39" s="2" t="n">
+        <v>-9.555642599999999</v>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>-35.7764813</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -708,6 +933,12 @@
           <t>Universidade Federal De Alagoas - Unnamed Road - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B40" s="2" t="n">
+        <v>-9.552133999999999</v>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>-35.77124999999999</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -715,6 +946,12 @@
           <t>Rua Senhor Do Bonfim 202 - Santos Dumont Maceió - Al 57018-530 Brasil</t>
         </is>
       </c>
+      <c r="B41" s="2" t="n">
+        <v>-9.5573503</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>-35.7825882</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -722,6 +959,12 @@
           <t>Br-104 1099 - Santos Dumont Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B42" s="2" t="n">
+        <v>-9.5564714</v>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>-35.7812506</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -729,6 +972,12 @@
           <t>Rua Santo Antônio 322 - Santos Dumont Maceió - Al República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B43" s="2" t="n">
+        <v>-9.5526211</v>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>-35.790461</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -736,6 +985,12 @@
           <t>R. Maurício De Melo E Mota 277-305 - Santos Dumont Maceió - Al 57075-655 Brasil</t>
         </is>
       </c>
+      <c r="B44" s="2" t="n">
+        <v>-9.5588791</v>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>-35.7853729</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -743,6 +998,12 @@
           <t>R. Maurício De Melo E Mota 539-575 - Santos Dumont Maceió - Al 57075-655 Brasil</t>
         </is>
       </c>
+      <c r="B45" s="2" t="n">
+        <v>-9.556795299999999</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>-35.7865437</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -750,6 +1011,12 @@
           <t>Av. Carnavalesco José Teofanes 124-162 - Santos Dumont Maceió - Al 57075-530 Brasil</t>
         </is>
       </c>
+      <c r="B46" s="2" t="n">
+        <v>-9.5581777</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>-35.78896170000001</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -757,6 +1024,12 @@
           <t>Av. Tancredo Neves 968-1002 - Santos Dumont Maceió - Al 57071-300 Brasil</t>
         </is>
       </c>
+      <c r="B47" s="2" t="n">
+        <v>-9.555773799999999</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>-35.7904942</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -764,6 +1037,12 @@
           <t>Av. Tancredo Neves 1200-1296 - Santos Dumont Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B48" s="2" t="n">
+        <v>-9.553751999999999</v>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>-35.7909765</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -771,6 +1050,12 @@
           <t>Av. Tancredo Neves 1442-1530 - Santos Dumont Maceió - Al 57071-300 Brasil</t>
         </is>
       </c>
+      <c r="B49" s="2" t="n">
+        <v>-9.551980499999999</v>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>-35.7901472</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -778,6 +1063,12 @@
           <t>R. Onélia Campêlo Da Paz 46-48 - Santos Dumont Maceió - Al 57075-720 Brasil</t>
         </is>
       </c>
+      <c r="B50" s="2" t="n">
+        <v>-9.551114</v>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>-35.7873119</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -785,6 +1076,12 @@
           <t>Rua Onélia Campelo Da Paz 202-208 - Santos Dumont Maceió - Al República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B51" s="2" t="n">
+        <v>-9.546662</v>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>-35.791912</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -792,6 +1089,12 @@
           <t>Rua Onélia Campelo Da Paz 103-123 - Santos Dumont Maceió - Al República Federativa Do Brasil</t>
         </is>
       </c>
+      <c r="B52" s="2" t="n">
+        <v>-9.5507568</v>
+      </c>
+      <c r="C52" s="2" t="n">
+        <v>-35.786958</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -799,6 +1102,12 @@
           <t>Terminal Santos Dumont - Cima</t>
         </is>
       </c>
+      <c r="B53" s="2" t="n">
+        <v>-22.9111438</v>
+      </c>
+      <c r="C53" s="2" t="n">
+        <v>-43.1648755</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -813,6 +1122,12 @@
           <t>Estrada Utinga 2-14 - Santos Dumont Maceió - Al 57100-000 Brasil</t>
         </is>
       </c>
+      <c r="B55" s="2" t="n">
+        <v>-9.5377907</v>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>-35.81515340000001</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -820,6 +1135,12 @@
           <t>Loteamento Betel 610</t>
         </is>
       </c>
+      <c r="B56" s="2" t="n">
+        <v>-9.540084199999999</v>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>-35.7965546</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -834,6 +1155,12 @@
           <t>Av. Dr. Fábio Wanderley 727-955 - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B58" s="2" t="n">
+        <v>-9.543493399999999</v>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>-35.7870338</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -841,12 +1168,24 @@
           <t>Avenida Doutor Fábio Wanderley 608-654 - Cidade Universitária Maceió - Al Brasil</t>
         </is>
       </c>
+      <c r="B59" s="2" t="n">
+        <v>-9.542950099999999</v>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>-35.7860535</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
           <t>Terminal Eustáquio Gomes</t>
         </is>
+      </c>
+      <c r="B60" s="2" t="n">
+        <v>-9.5418305</v>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>-35.7832275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>